<commit_message>
:large_blue_diamond: feat(doc): Doc update
+ Rapport
+ Work diary
</commit_message>
<xml_diff>
--- a/matvelickov-journalTravail-webstore.xlsx
+++ b/matvelickov-journalTravail-webstore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\node-webstore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469FA19-B73D-4899-B6B1-86F4EFED78E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339DC1BA-CB50-4DE2-BCC5-70D188FB87B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="2895" yWindow="480" windowWidth="21600" windowHeight="11835" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -135,10 +135,67 @@
     <t>Création des documents : rapport, journal de travail.</t>
   </si>
   <si>
-    <t>Documentation sur les routes et les controllers.</t>
+    <t>Mise en place de l'environnement du projet (Docker, Node, Documents).</t>
   </si>
   <si>
-    <t>Mise en place de l'environnement du projet (Docker, Node, Documents).</t>
+    <t>Génération d'un certificat auto-signé OpenSSL et redirection sur une page sécurisée (HTTPS).</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6I2vRDawshA</t>
+  </si>
+  <si>
+    <t>Création d'un mock user et création de routes GET pour la récupération des utilisateurs.</t>
+  </si>
+  <si>
+    <t>Renseignement sur les routes et les controllers.</t>
+  </si>
+  <si>
+    <t>Renseignement sur le fonctionnement des routes et de la fonction .find() avec les controllers.</t>
+  </si>
+  <si>
+    <t>Connexion à la base de données.</t>
+  </si>
+  <si>
+    <t>Création de la route GET /users/.</t>
+  </si>
+  <si>
+    <t>Création de la route GET /users/:name.</t>
+  </si>
+  <si>
+    <t>Renseignement sur la connexion à la base de données.</t>
+  </si>
+  <si>
+    <t>Création de la route POST /users/login.</t>
+  </si>
+  <si>
+    <t>Développement de la route de connexion avec le token.</t>
+  </si>
+  <si>
+    <t>Développement du rapport.</t>
+  </si>
+  <si>
+    <t>Avancement dans la création de la route de connexion.</t>
+  </si>
+  <si>
+    <t>Documentation du projet.</t>
+  </si>
+  <si>
+    <t>Configuration du port du serveur sur 443.</t>
+  </si>
+  <si>
+    <t>Création de la clé privée pour la création du token.</t>
+  </si>
+  <si>
+    <t>Création de l'interface visuelle du projet (HTML).</t>
+  </si>
+  <si>
+    <t>Finalisation de l'interface utilisateur</t>
+  </si>
+  <si>
+    <t>Finalisation du login de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Connexion à la base de données afin de récupérer les données depuis cette dernière.</t>
   </si>
 </sst>
 </file>
@@ -153,7 +210,7 @@
     <numFmt numFmtId="168" formatCode="00\ &quot;min&quot;"/>
     <numFmt numFmtId="169" formatCode="hh\ &quot;h&quot;\ mm\ &quot;min&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,6 +285,22 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -319,10 +392,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -417,13 +491,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -435,8 +502,19 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -1041,25 +1119,25 @@
                   <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0.60069444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.2916666666666671E-2</c:v>
+                  <c:v>6.5972222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.2916666666666671E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,9 +2048,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2007,11 +2085,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2025,7 +2103,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heures "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heures 10 minutes</v>
+        <v>0 jours 19 heures 0 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2040,24 +2118,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>420</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>130</v>
+        <v>720</v>
       </c>
       <c r="E4" s="49">
         <f>SUM(C4:D4)</f>
-        <v>190</v>
+        <v>1140</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="21" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -2087,7 +2165,7 @@
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
         <v>13</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="54">
         <v>45378</v>
       </c>
       <c r="C7" s="32"/>
@@ -2107,7 +2185,7 @@
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
         <v>13</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="56">
         <v>45378</v>
       </c>
       <c r="C8" s="33"/>
@@ -2117,8 +2195,8 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="54" t="s">
-        <v>32</v>
+      <c r="F8" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
@@ -2136,7 +2214,7 @@
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
         <v>13</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="54">
         <v>45378</v>
       </c>
       <c r="C9" s="34">
@@ -2146,10 +2224,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="55" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>35</v>
       </c>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
@@ -2167,7 +2245,7 @@
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
         <v>13</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="56">
         <v>45378</v>
       </c>
       <c r="C10" s="33"/>
@@ -2175,7 +2253,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F10" s="45" t="s">
         <v>30</v>
@@ -2192,16 +2270,28 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="str">
+      <c r="A11" s="8">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="54">
+        <v>45399</v>
+      </c>
+      <c r="C11" s="34">
+        <v>2</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>33</v>
+      </c>
       <c r="M11" t="s">
         <v>6</v>
       </c>
@@ -2213,14 +2303,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="40"/>
-      <c r="F12" s="45"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="55">
+        <v>45399</v>
+      </c>
+      <c r="C12" s="33">
+        <v>1</v>
+      </c>
+      <c r="D12" s="40">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2233,15 +2334,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="str">
+      <c r="A13" s="8">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="56"/>
+        <v>17</v>
+      </c>
+      <c r="B13" s="54">
+        <v>45406</v>
+      </c>
       <c r="C13" s="34"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="45"/>
+      <c r="D13" s="41">
+        <v>45</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="18"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2254,14 +2363,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="58"/>
+        <v>17</v>
+      </c>
+      <c r="B14" s="56">
+        <v>45406</v>
+      </c>
       <c r="C14" s="33"/>
-      <c r="D14" s="40"/>
-      <c r="F14" s="45"/>
+      <c r="D14" s="40">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>38</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>24</v>
@@ -2274,15 +2392,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="str">
+      <c r="A15" s="8">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="37">
+        <v>45406</v>
+      </c>
       <c r="C15" s="34"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="45"/>
+      <c r="D15" s="41">
+        <v>30</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>39</v>
+      </c>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>25</v>
@@ -2295,164 +2421,281 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="36"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="36">
+        <v>45406</v>
+      </c>
       <c r="C16" s="33"/>
-      <c r="D16" s="40"/>
-      <c r="F16" s="45"/>
+      <c r="D16" s="40">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>40</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="str">
+      <c r="A17" s="8">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="37">
+        <v>45406</v>
+      </c>
       <c r="C17" s="34"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="45"/>
+      <c r="D17" s="41">
+        <v>55</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="36">
+        <v>45413</v>
+      </c>
       <c r="C18" s="33"/>
-      <c r="D18" s="40"/>
-      <c r="F18" s="45"/>
+      <c r="D18" s="40">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="str">
+      <c r="A19" s="8">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="45"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="36">
+        <v>45413</v>
+      </c>
+      <c r="C19" s="34">
+        <v>1</v>
+      </c>
+      <c r="D19" s="41">
+        <v>30</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>42</v>
+      </c>
       <c r="G19" s="18"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="36">
+        <v>45413</v>
+      </c>
       <c r="C20" s="33"/>
-      <c r="D20" s="40"/>
-      <c r="F20" s="45"/>
+      <c r="D20" s="40">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>43</v>
+      </c>
       <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="str">
+      <c r="A21" s="8">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="37"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="37">
+        <v>45413</v>
+      </c>
       <c r="C21" s="34"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="45"/>
+      <c r="D21" s="41">
+        <v>40</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>44</v>
+      </c>
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="36">
+        <v>45420</v>
+      </c>
       <c r="C22" s="33"/>
-      <c r="D22" s="40"/>
-      <c r="F22" s="45"/>
+      <c r="D22" s="40">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>46</v>
+      </c>
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="str">
+      <c r="A23" s="8">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="37"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="36">
+        <v>45420</v>
+      </c>
       <c r="C23" s="34"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="45"/>
+      <c r="D23" s="41">
+        <v>40</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="40"/>
-      <c r="F24" s="45"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="36">
+        <v>45420</v>
+      </c>
+      <c r="C24" s="33">
+        <v>1</v>
+      </c>
+      <c r="D24" s="40">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>48</v>
+      </c>
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="str">
+      <c r="A25" s="8">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="37"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="37">
+        <v>45420</v>
+      </c>
       <c r="C25" s="34"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="45"/>
+      <c r="D25" s="41">
+        <v>50</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="40"/>
-      <c r="F26" s="45"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="36">
+        <v>45427</v>
+      </c>
+      <c r="C26" s="33">
+        <v>1</v>
+      </c>
+      <c r="D26" s="40">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>49</v>
+      </c>
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="str">
+      <c r="A27" s="8">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="37"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="37">
+        <v>45427</v>
+      </c>
       <c r="C27" s="34"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="45"/>
+      <c r="D27" s="41">
+        <v>50</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>50</v>
+      </c>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="36"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="36">
+        <v>45427</v>
+      </c>
       <c r="C28" s="33"/>
-      <c r="D28" s="40"/>
-      <c r="F28" s="44"/>
+      <c r="D28" s="40">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>51</v>
+      </c>
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8294,10 +8537,13 @@
       <formula1>$M$7:$M$15</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{57412A94-F88B-44FE-B9B5-66DBFCE5B68C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8354,11 +8600,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>505</v>
       </c>
       <c r="C5" s="50" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8366,7 +8612,7 @@
       </c>
       <c r="D5" s="42">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>3.125E-2</v>
+        <v>0.60069444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8390,11 +8636,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8402,7 +8648,7 @@
       </c>
       <c r="D7" s="42">
         <f t="shared" si="0"/>
-        <v>7.2916666666666671E-2</v>
+        <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8430,7 +8676,7 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C9" s="35" t="str">
         <f>'Journal de travail'!M13</f>
@@ -8438,7 +8684,7 @@
       </c>
       <c r="D9" s="42">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -8458,7 +8704,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="C11" s="48" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8466,7 +8712,7 @@
       </c>
       <c r="D11" s="42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8475,7 +8721,7 @@
       </c>
       <c r="D12" s="43">
         <f>SUM(D4:D11)</f>
-        <v>0.13194444444444445</v>
+        <v>0.74999999999999989</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8754,15 +9000,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8772,6 +9009,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8795,14 +9041,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8814,4 +9052,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>